<commit_message>
transition du format xlsx au format tsv
</commit_message>
<xml_diff>
--- a/documentation/analyse/correspondance_champs_ancien-nouveau_schémas.xlsx
+++ b/documentation/analyse/correspondance_champs_ancien-nouveau_schémas.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="116">
   <si>
     <t>Ancien Schéma</t>
   </si>
@@ -65,9 +65,6 @@
     <t>DATE_MODIFICATION</t>
   </si>
   <si>
-    <t>ILTAPTZ</t>
-  </si>
-  <si>
     <t>ILTADTN</t>
   </si>
   <si>
@@ -80,9 +77,6 @@
     <t>LONGUEUR</t>
   </si>
   <si>
-    <t>CCODDFT</t>
-  </si>
-  <si>
     <t>VOIECVT</t>
   </si>
   <si>
@@ -110,12 +104,6 @@
     <t>FID_TRONCON</t>
   </si>
   <si>
-    <t>CDTMCVT</t>
-  </si>
-  <si>
-    <t>CDTSCVT</t>
-  </si>
-  <si>
     <t>TA_RELATION_TRONCON_VOIE_LOG</t>
   </si>
   <si>
@@ -225,12 +213,6 @@
   </si>
   <si>
     <t>COMPLEMENT_NUMERO_SEUIL</t>
-  </si>
-  <si>
-    <t>CXLAPTZ</t>
-  </si>
-  <si>
-    <t>CYLAPTZ</t>
   </si>
   <si>
     <t>START_POINT
@@ -352,18 +334,6 @@
 et ce sera un champ virtuel qui calculera automatiquemet le code INSEE de chaque seuil via une requête spatiale.</t>
   </si>
   <si>
-    <t>Date de saisie de la géométrie du seuil en base (un point pourra disposer de plusieurs seuils contenus dans TA_INFOS_SEUIL). Cette date est et sera remplie automatiquement.</t>
-  </si>
-  <si>
-    <t>Date de modification de la géométrie du seuil en base. Cette date est et sera remplie automatiquement.</t>
-  </si>
-  <si>
-    <t>Date de modification des informations du seuil en base. Cette date est et sera remplie automatiquement.</t>
-  </si>
-  <si>
-    <t>Date de saisie des informations du seuil en base. Cette date est et sera remplie automatiquement.</t>
-  </si>
-  <si>
     <t>Numéro de la parcelle (ISSU du parcellaire cadastral) dans laquelle se situe le seuil.</t>
   </si>
   <si>
@@ -387,6 +357,38 @@
   </si>
   <si>
     <t>Code côté du tronçon (droite ou gauche) sur lequel se situe le seuil. Les côtés sont déterminés par rapport au sens de codage des tronçons, et non par rapport au sens de circulation. Cette information sera conservée dans le nouveau schéma.</t>
+  </si>
+  <si>
+    <t>CCODDFT
+CXLAPTZ
+CYLAPTZ</t>
+  </si>
+  <si>
+    <t>CDTSCVT
+CDTMCVT</t>
+  </si>
+  <si>
+    <t>ILTASIT
+ILTASEU</t>
+  </si>
+  <si>
+    <t>TA_SEUIL
+TA_INFOS_SEUIL</t>
+  </si>
+  <si>
+    <t>DATE_SAISIE
+DATE_SAISIE</t>
+  </si>
+  <si>
+    <t>DATE_MODIFICATION
+DATE_MODIFICATION</t>
+  </si>
+  <si>
+    <t>Dates de modification de la géométrie et des informations du seuil en base. Ces dates sont et seront remplies automatiquement.</t>
+  </si>
+  <si>
+    <t>Dates de saisie de la géométrie et des informations du seuil en base (un point pourra disposer de plusieurs seuils contenus dans TA_INFOS_SEUIL). 
+Ces dates sont et seront remplies automatiquement.</t>
   </si>
 </sst>
 </file>
@@ -567,7 +569,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -614,8 +616,33 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -623,46 +650,39 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -949,10 +969,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E45"/>
+  <dimension ref="A1:E39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32:C33"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection sqref="A1:E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -964,14 +984,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="21" t="s">
+      <c r="B1" s="31"/>
+      <c r="C1" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="22"/>
+      <c r="D1" s="31"/>
       <c r="E1" s="2"/>
     </row>
     <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -988,7 +1008,7 @@
         <v>2</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1005,7 +1025,7 @@
         <v>7</v>
       </c>
       <c r="E3" s="16" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1022,7 +1042,7 @@
         <v>8</v>
       </c>
       <c r="E4" s="17" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1039,7 +1059,7 @@
         <v>10</v>
       </c>
       <c r="E5" s="16" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1056,7 +1076,7 @@
         <v>12</v>
       </c>
       <c r="E6" s="17" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1064,635 +1084,552 @@
         <v>4</v>
       </c>
       <c r="B7" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="D7" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="6" t="s">
-        <v>17</v>
-      </c>
       <c r="E7" s="16" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>5</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="E8" s="17" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D9" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="B9" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>76</v>
-      </c>
       <c r="E9" s="16" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="C10" s="23" t="s">
-        <v>74</v>
-      </c>
-      <c r="D10" s="30" t="s">
-        <v>77</v>
-      </c>
-      <c r="E10" s="24" t="s">
-        <v>116</v>
+        <v>66</v>
+      </c>
+      <c r="C10" s="28" t="s">
+        <v>68</v>
+      </c>
+      <c r="D10" s="29" t="s">
+        <v>71</v>
+      </c>
+      <c r="E10" s="32" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="C11" s="23"/>
-      <c r="D11" s="30"/>
-      <c r="E11" s="25"/>
+        <v>67</v>
+      </c>
+      <c r="C11" s="28"/>
+      <c r="D11" s="29"/>
+      <c r="E11" s="33"/>
     </row>
     <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B12" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="E12" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="C12" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="D12" s="10" t="s">
+    </row>
+    <row r="13" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="36" t="s">
+        <v>108</v>
+      </c>
+      <c r="C13" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="35" t="s">
+        <v>63</v>
+      </c>
+      <c r="E13" s="23" t="s">
         <v>79</v>
       </c>
-      <c r="E12" s="18" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" s="8" t="s">
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="D13" s="30" t="s">
-        <v>69</v>
-      </c>
-      <c r="E13" s="26" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="C14" s="23"/>
-      <c r="D14" s="30"/>
-      <c r="E14" s="27"/>
+      <c r="D14" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E14" s="16" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="C15" s="23"/>
-      <c r="D15" s="30"/>
-      <c r="E15" s="27"/>
+        <v>21</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E15" s="17" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E16" s="16" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E17" s="17" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D18" s="6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="37" t="s">
+        <v>109</v>
+      </c>
+      <c r="C18" s="38" t="s">
         <v>26</v>
       </c>
-      <c r="E18" s="16" t="s">
-        <v>88</v>
+      <c r="D18" s="39" t="s">
+        <v>71</v>
+      </c>
+      <c r="E18" s="19" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="B19" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E19" s="17" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="E20" s="18" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E21" s="17" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E22" s="16" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E23" s="17" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E24" s="16" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E25" s="17" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E26" s="18" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="E27" s="17" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="B28" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="C28" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="D28" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="E28" s="18" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="40" t="s">
+        <v>110</v>
+      </c>
+      <c r="B29" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="C19" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D19" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="E19" s="17" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C20" s="28" t="s">
-        <v>30</v>
-      </c>
-      <c r="D20" s="29" t="s">
-        <v>77</v>
-      </c>
-      <c r="E20" s="19" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C21" s="28"/>
-      <c r="D21" s="29"/>
-      <c r="E21" s="20"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="B22" s="8" t="s">
+      <c r="C29" s="34" t="s">
+        <v>44</v>
+      </c>
+      <c r="D29" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="C22" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="D22" s="8" t="s">
+      <c r="E29" s="24" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D30" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E22" s="17" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A23" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="B23" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="C23" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="D23" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="E23" s="18" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="B24" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="C24" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="D24" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="E24" s="17" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B25" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D25" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="E25" s="16" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="B26" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="C26" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="D26" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E26" s="17" t="s">
+      <c r="E30" s="16" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B27" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D27" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E27" s="16" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="B28" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="C28" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="D28" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="E28" s="17" t="s">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E31" s="17" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B29" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="D29" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="E29" s="18" t="s">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E32" s="16" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="7" t="s">
+    <row r="33" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="B33" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="C33" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="B30" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="C30" s="7" t="s">
+      <c r="D33" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="E33" s="23" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="D30" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="E30" s="17" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="B31" s="14" t="s">
+      <c r="B34" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="C31" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="D31" s="14" t="s">
+      <c r="C34" s="41" t="s">
+        <v>111</v>
+      </c>
+      <c r="D34" s="37" t="s">
+        <v>112</v>
+      </c>
+      <c r="E34" s="42" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="B35" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="E31" s="18" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="B32" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C32" s="23" t="s">
-        <v>48</v>
-      </c>
-      <c r="D32" s="30" t="s">
-        <v>27</v>
-      </c>
-      <c r="E32" s="32" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="B33" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C33" s="23"/>
-      <c r="D33" s="30"/>
-      <c r="E33" s="33"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="B34" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="D34" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E34" s="16" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="B35" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C35" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="D35" s="8" t="s">
-        <v>8</v>
+      <c r="C35" s="40" t="s">
+        <v>111</v>
+      </c>
+      <c r="D35" s="36" t="s">
+        <v>113</v>
       </c>
       <c r="E35" s="17" t="s">
-        <v>103</v>
+        <v>114</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="E36" s="16" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A37" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="B37" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="C37" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="D37" s="12" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C37" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="E37" s="31" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="28" t="s">
-        <v>52</v>
-      </c>
-      <c r="B38" s="29" t="s">
-        <v>58</v>
-      </c>
-      <c r="C38" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="D38" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E38" s="16" t="s">
-        <v>106</v>
+      <c r="D37" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="E37" s="17" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="B38" s="26" t="s">
+        <v>61</v>
+      </c>
+      <c r="C38" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="D38" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="E38" s="27" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="28"/>
-      <c r="B39" s="29"/>
-      <c r="C39" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="D39" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E39" s="16" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="23" t="s">
-        <v>52</v>
-      </c>
-      <c r="B40" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="C40" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="D40" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="E40" s="17" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="23"/>
-      <c r="B41" s="30"/>
-      <c r="C41" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="D41" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="E41" s="17" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="B42" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="C42" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="D42" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="E42" s="16" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="B43" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="C43" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="D43" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="E43" s="17" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="34" t="s">
-        <v>52</v>
-      </c>
-      <c r="B44" s="35" t="s">
-        <v>65</v>
-      </c>
-      <c r="C44" s="34" t="s">
-        <v>61</v>
-      </c>
-      <c r="D44" s="35" t="s">
-        <v>66</v>
-      </c>
-      <c r="E44" s="36" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="1"/>
-      <c r="B45" s="1"/>
-      <c r="C45" s="1"/>
-      <c r="D45" s="1"/>
+      <c r="A39" s="1"/>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="18">
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="A40:A41"/>
-    <mergeCell ref="B40:B41"/>
-    <mergeCell ref="E32:E33"/>
+  <mergeCells count="5">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="C10:C11"/>
     <mergeCell ref="E10:E11"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="E13:E15"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="D32:D33"/>
-    <mergeCell ref="C13:C15"/>
-    <mergeCell ref="D13:D15"/>
-    <mergeCell ref="D20:D21"/>
     <mergeCell ref="D10:D11"/>
-    <mergeCell ref="C20:C21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
ajout d'un ";" pour séparer les valeurs concaténées.
</commit_message>
<xml_diff>
--- a/documentation/analyse/correspondance_champs_ancien-nouveau_schémas.xlsx
+++ b/documentation/analyse/correspondance_champs_ancien-nouveau_schémas.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="117">
   <si>
     <t>Ancien Schéma</t>
   </si>
@@ -225,9 +225,6 @@
     <t>TRCPERE</t>
   </si>
   <si>
-    <t>CDTSFILIA</t>
-  </si>
-  <si>
     <t>CDTMFILIA</t>
   </si>
   <si>
@@ -359,27 +356,10 @@
     <t>Code côté du tronçon (droite ou gauche) sur lequel se situe le seuil. Les côtés sont déterminés par rapport au sens de codage des tronçons, et non par rapport au sens de circulation. Cette information sera conservée dans le nouveau schéma.</t>
   </si>
   <si>
-    <t>CCODDFT
-CXLAPTZ
-CYLAPTZ</t>
-  </si>
-  <si>
-    <t>CDTSCVT
-CDTMCVT</t>
-  </si>
-  <si>
-    <t>ILTASIT
-ILTASEU</t>
-  </si>
-  <si>
     <t>TA_SEUIL
 TA_INFOS_SEUIL</t>
   </si>
   <si>
-    <t>DATE_SAISIE
-DATE_SAISIE</t>
-  </si>
-  <si>
     <t>DATE_MODIFICATION
 DATE_MODIFICATION</t>
   </si>
@@ -389,6 +369,30 @@
   <si>
     <t>Dates de saisie de la géométrie et des informations du seuil en base (un point pourra disposer de plusieurs seuils contenus dans TA_INFOS_SEUIL). 
 Ces dates sont et seront remplies automatiquement.</t>
+  </si>
+  <si>
+    <t>TA_SEUIL ; 
+TA_INFOS_SEUIL</t>
+  </si>
+  <si>
+    <t>ILTASIT ; 
+ILTASEU</t>
+  </si>
+  <si>
+    <t>DATE_SAISIE ; 
+DATE_SAISIE</t>
+  </si>
+  <si>
+    <t>CDTSCVT ; 
+CDTMCVT</t>
+  </si>
+  <si>
+    <t>CCODDFT ; 
+CXLAPTZ ; 
+CYLAPTZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CDTSFILIA ; </t>
   </si>
 </sst>
 </file>
@@ -639,49 +643,49 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -971,8 +975,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection sqref="A1:E38"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -984,14 +988,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="30" t="s">
+      <c r="B1" s="38"/>
+      <c r="C1" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="31"/>
+      <c r="D1" s="38"/>
       <c r="E1" s="2"/>
     </row>
     <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -1008,7 +1012,7 @@
         <v>2</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1025,7 +1029,7 @@
         <v>7</v>
       </c>
       <c r="E3" s="16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1042,7 +1046,7 @@
         <v>8</v>
       </c>
       <c r="E4" s="17" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1059,7 +1063,7 @@
         <v>10</v>
       </c>
       <c r="E5" s="16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1076,7 +1080,7 @@
         <v>12</v>
       </c>
       <c r="E6" s="17" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1093,7 +1097,7 @@
         <v>16</v>
       </c>
       <c r="E7" s="16" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1104,13 +1108,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="D8" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="D8" s="8" t="s">
-        <v>69</v>
-      </c>
       <c r="E8" s="17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1121,13 +1125,13 @@
         <v>65</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E9" s="16" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1135,16 +1139,16 @@
         <v>64</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="C10" s="28" t="s">
-        <v>68</v>
-      </c>
-      <c r="D10" s="29" t="s">
-        <v>71</v>
-      </c>
-      <c r="E10" s="32" t="s">
-        <v>106</v>
+        <v>116</v>
+      </c>
+      <c r="C10" s="39" t="s">
+        <v>67</v>
+      </c>
+      <c r="D10" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="E10" s="40" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1152,44 +1156,44 @@
         <v>64</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="C11" s="28"/>
-      <c r="D11" s="29"/>
-      <c r="E11" s="33"/>
+        <v>66</v>
+      </c>
+      <c r="C11" s="39"/>
+      <c r="D11" s="42"/>
+      <c r="E11" s="41"/>
     </row>
     <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>64</v>
       </c>
       <c r="B12" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="D12" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="C12" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>73</v>
-      </c>
       <c r="E12" s="18" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="36" t="s">
-        <v>108</v>
-      </c>
-      <c r="C13" s="34" t="s">
+      <c r="B13" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="C13" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="D13" s="35" t="s">
+      <c r="D13" s="29" t="s">
         <v>63</v>
       </c>
       <c r="E13" s="23" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -1206,7 +1210,7 @@
         <v>20</v>
       </c>
       <c r="E14" s="16" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -1223,7 +1227,7 @@
         <v>22</v>
       </c>
       <c r="E15" s="17" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -1240,7 +1244,7 @@
         <v>24</v>
       </c>
       <c r="E16" s="16" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -1257,24 +1261,24 @@
         <v>25</v>
       </c>
       <c r="E17" s="17" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="37" t="s">
-        <v>109</v>
-      </c>
-      <c r="C18" s="38" t="s">
+      <c r="B18" s="31" t="s">
+        <v>114</v>
+      </c>
+      <c r="C18" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="D18" s="39" t="s">
-        <v>71</v>
+      <c r="D18" s="33" t="s">
+        <v>70</v>
       </c>
       <c r="E18" s="19" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -1291,7 +1295,7 @@
         <v>7</v>
       </c>
       <c r="E19" s="17" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -1308,7 +1312,7 @@
         <v>31</v>
       </c>
       <c r="E20" s="18" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -1325,7 +1329,7 @@
         <v>33</v>
       </c>
       <c r="E21" s="17" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -1342,7 +1346,7 @@
         <v>35</v>
       </c>
       <c r="E22" s="16" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -1359,7 +1363,7 @@
         <v>10</v>
       </c>
       <c r="E23" s="17" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -1376,7 +1380,7 @@
         <v>12</v>
       </c>
       <c r="E24" s="16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -1393,7 +1397,7 @@
         <v>39</v>
       </c>
       <c r="E25" s="17" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1410,7 +1414,7 @@
         <v>42</v>
       </c>
       <c r="E26" s="18" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -1427,7 +1431,7 @@
         <v>47</v>
       </c>
       <c r="E27" s="17" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1444,24 +1448,24 @@
         <v>51</v>
       </c>
       <c r="E28" s="18" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="40" t="s">
-        <v>110</v>
+      <c r="A29" s="34" t="s">
+        <v>112</v>
       </c>
       <c r="B29" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="C29" s="34" t="s">
+      <c r="C29" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="D29" s="35" t="s">
+      <c r="D29" s="29" t="s">
         <v>25</v>
       </c>
       <c r="E29" s="24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -1478,7 +1482,7 @@
         <v>7</v>
       </c>
       <c r="E30" s="16" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -1495,7 +1499,7 @@
         <v>8</v>
       </c>
       <c r="E31" s="17" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -1512,7 +1516,7 @@
         <v>51</v>
       </c>
       <c r="E32" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1529,24 +1533,24 @@
         <v>53</v>
       </c>
       <c r="E33" s="23" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="38" t="s">
+      <c r="A34" s="32" t="s">
         <v>48</v>
       </c>
-      <c r="B34" s="39" t="s">
+      <c r="B34" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="C34" s="41" t="s">
+      <c r="C34" s="35" t="s">
         <v>111</v>
       </c>
-      <c r="D34" s="37" t="s">
-        <v>112</v>
-      </c>
-      <c r="E34" s="42" t="s">
-        <v>115</v>
+      <c r="D34" s="31" t="s">
+        <v>113</v>
+      </c>
+      <c r="E34" s="36" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1556,14 +1560,14 @@
       <c r="B35" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="C35" s="40" t="s">
-        <v>111</v>
-      </c>
-      <c r="D35" s="36" t="s">
-        <v>113</v>
+      <c r="C35" s="34" t="s">
+        <v>107</v>
+      </c>
+      <c r="D35" s="30" t="s">
+        <v>108</v>
       </c>
       <c r="E35" s="17" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -1580,7 +1584,7 @@
         <v>58</v>
       </c>
       <c r="E36" s="16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -1597,7 +1601,7 @@
         <v>60</v>
       </c>
       <c r="E37" s="17" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1614,7 +1618,7 @@
         <v>62</v>
       </c>
       <c r="E38" s="27" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
remplacement du ";" par un "-" car le ";" est utilisé pour séparer les cellules.
</commit_message>
<xml_diff>
--- a/documentation/analyse/correspondance_champs_ancien-nouveau_schémas.xlsx
+++ b/documentation/analyse/correspondance_champs_ancien-nouveau_schémas.xlsx
@@ -371,28 +371,28 @@
 Ces dates sont et seront remplies automatiquement.</t>
   </si>
   <si>
-    <t>TA_SEUIL ; 
+    <t xml:space="preserve">CDTSFILIA - </t>
+  </si>
+  <si>
+    <t>CCODDFT - 
+CXLAPTZ - 
+CYLAPTZ</t>
+  </si>
+  <si>
+    <t>CDTSCVT - 
+CDTMCVT</t>
+  </si>
+  <si>
+    <t>ILTASIT - 
+ILTASEU</t>
+  </si>
+  <si>
+    <t>TA_SEUIL - 
 TA_INFOS_SEUIL</t>
   </si>
   <si>
-    <t>ILTASIT ; 
-ILTASEU</t>
-  </si>
-  <si>
-    <t>DATE_SAISIE ; 
+    <t>DATE_SAISIE - 
 DATE_SAISIE</t>
-  </si>
-  <si>
-    <t>CDTSCVT ; 
-CDTMCVT</t>
-  </si>
-  <si>
-    <t>CCODDFT ; 
-CXLAPTZ ; 
-CYLAPTZ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CDTSFILIA ; </t>
   </si>
 </sst>
 </file>
@@ -975,8 +975,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1139,7 +1139,7 @@
         <v>64</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="C10" s="39" t="s">
         <v>67</v>
@@ -1184,7 +1184,7 @@
         <v>13</v>
       </c>
       <c r="B13" s="30" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C13" s="28" t="s">
         <v>15</v>
@@ -1269,7 +1269,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="31" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C18" s="32" t="s">
         <v>26</v>
@@ -1453,7 +1453,7 @@
     </row>
     <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="34" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B29" s="22" t="s">
         <v>5</v>
@@ -1544,10 +1544,10 @@
         <v>54</v>
       </c>
       <c r="C34" s="35" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="D34" s="31" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="E34" s="36" t="s">
         <v>110</v>

</xml_diff>

<commit_message>
remplacement - par /
</commit_message>
<xml_diff>
--- a/documentation/analyse/correspondance_champs_ancien-nouveau_schémas.xlsx
+++ b/documentation/analyse/correspondance_champs_ancien-nouveau_schémas.xlsx
@@ -368,29 +368,29 @@
 Ces dates sont et seront remplies automatiquement.</t>
   </si>
   <si>
-    <t>CCODDFT - 
-CXLAPTZ - 
+    <t>CDTSFILIA / 
+CDTMFILIA</t>
+  </si>
+  <si>
+    <t>CCODDFT / 
+CXLAPTZ / 
 CYLAPTZ</t>
   </si>
   <si>
-    <t>CDTSCVT - 
+    <t>CDTSCVT / 
 CDTMCVT</t>
   </si>
   <si>
-    <t>ILTASIT - 
+    <t>ILTASIT / 
 ILTASEU</t>
   </si>
   <si>
-    <t>TA_SEUIL - 
+    <t>TA_SEUIL / 
 TA_INFOS_SEUIL</t>
   </si>
   <si>
-    <t>DATE_SAISIE - 
+    <t>DATE_SAISIE / 
 DATE_SAISIE</t>
-  </si>
-  <si>
-    <t>CDTSFILIA - 
-CDTMFILIA</t>
   </si>
 </sst>
 </file>
@@ -673,14 +673,14 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -971,7 +971,7 @@
   <dimension ref="A1:E38"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -983,14 +983,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="39" t="s">
+      <c r="B1" s="41"/>
+      <c r="C1" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="40"/>
+      <c r="D1" s="41"/>
       <c r="E1" s="2"/>
     </row>
     <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -1134,7 +1134,7 @@
         <v>64</v>
       </c>
       <c r="B10" s="30" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="C10" s="37" t="s">
         <v>66</v>
@@ -1142,7 +1142,7 @@
       <c r="D10" s="38" t="s">
         <v>69</v>
       </c>
-      <c r="E10" s="41" t="s">
+      <c r="E10" s="39" t="s">
         <v>104</v>
       </c>
     </row>
@@ -1168,7 +1168,7 @@
         <v>13</v>
       </c>
       <c r="B12" s="30" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C12" s="28" t="s">
         <v>15</v>
@@ -1253,7 +1253,7 @@
         <v>17</v>
       </c>
       <c r="B17" s="31" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C17" s="32" t="s">
         <v>26</v>
@@ -1437,7 +1437,7 @@
     </row>
     <row r="28" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="34" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B28" s="22" t="s">
         <v>5</v>
@@ -1528,10 +1528,10 @@
         <v>54</v>
       </c>
       <c r="C33" s="35" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D33" s="31" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E33" s="36" t="s">
         <v>109</v>

</xml_diff>